<commit_message>
working mysql database programs
</commit_message>
<xml_diff>
--- a/Technical Fresher Training-Course Content.xlsx
+++ b/Technical Fresher Training-Course Content.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\A5ABO0UA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\javabasics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DACD7E60-E3B6-6641-B7F9-33B3F68FC408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{527CB0AB-7998-47C7-84EC-15606664CBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Fresher Training" sheetId="5" r:id="rId1"/>
     <sheet name="Java Basics" sheetId="1" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="6" r:id="rId3"/>
+    <sheet name="Score Sheet-Java Basics" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,19 +26,72 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>skillwiseuser1</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{E13995B3-BF21-4FD5-B92A-28D6DACC2FBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scale of  1 - 5
+1- Poor
+2 - Average
+3 - Above Average
+4 - Good
+5 - Outstanding</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{5E9B5F7B-084C-4492-9445-ABE6359961D4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scores out of 100</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{B2D723B4-EC91-453F-9992-11C1DA218DE0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scores out of 100</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="239">
   <si>
     <t>Object-Oriented Programming Concepts</t>
   </si>
@@ -492,13 +547,274 @@
   </si>
   <si>
     <t>Total Duration in Hours</t>
+  </si>
+  <si>
+    <t>Duration in Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Date </t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Timing</t>
+  </si>
+  <si>
+    <t>Day1</t>
+  </si>
+  <si>
+    <t>Day2</t>
+  </si>
+  <si>
+    <t>Day3</t>
+  </si>
+  <si>
+    <t>Day4</t>
+  </si>
+  <si>
+    <t>Day5</t>
+  </si>
+  <si>
+    <t>Day6</t>
+  </si>
+  <si>
+    <t>Day7</t>
+  </si>
+  <si>
+    <t>Day8</t>
+  </si>
+  <si>
+    <t>Day9</t>
+  </si>
+  <si>
+    <t>Day10</t>
+  </si>
+  <si>
+    <t>Day11</t>
+  </si>
+  <si>
+    <t>Day12</t>
+  </si>
+  <si>
+    <t>Day13</t>
+  </si>
+  <si>
+    <t>Day14</t>
+  </si>
+  <si>
+    <t>Day15</t>
+  </si>
+  <si>
+    <t>Day16</t>
+  </si>
+  <si>
+    <t>Day17</t>
+  </si>
+  <si>
+    <t>Day18</t>
+  </si>
+  <si>
+    <t>Day19</t>
+  </si>
+  <si>
+    <t>Day20</t>
+  </si>
+  <si>
+    <t>Day21</t>
+  </si>
+  <si>
+    <t>Day22</t>
+  </si>
+  <si>
+    <t>Day23</t>
+  </si>
+  <si>
+    <t>Day24</t>
+  </si>
+  <si>
+    <t>Day25</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>9.00AM to 2.00PM IST</t>
+  </si>
+  <si>
+    <t>Trainer Name</t>
+  </si>
+  <si>
+    <t>Kannan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekend </t>
+  </si>
+  <si>
+    <t>Long Weekend</t>
+  </si>
+  <si>
+    <t>Postponed</t>
+  </si>
+  <si>
+    <t>Anjaneyulu</t>
+  </si>
+  <si>
+    <t>Public Holiday</t>
+  </si>
+  <si>
+    <t>S. No</t>
+  </si>
+  <si>
+    <t>Participants Name</t>
+  </si>
+  <si>
+    <t>Trainer's Feedback Creteria</t>
+  </si>
+  <si>
+    <t>Assessment Scores</t>
+  </si>
+  <si>
+    <t>Assignment Scores</t>
+  </si>
+  <si>
+    <t>Time Punctuality</t>
+  </si>
+  <si>
+    <t>Active Attentiveness</t>
+  </si>
+  <si>
+    <t>Interaction Level</t>
+  </si>
+  <si>
+    <t>Query Raising</t>
+  </si>
+  <si>
+    <t>Level of Understanding</t>
+  </si>
+  <si>
+    <t>Hands on Performance</t>
+  </si>
+  <si>
+    <t>Topic Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divya Kalyani, Pedapudi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kambhampati, Yasaswi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kothem, Sri Satya Trinadh lokesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilla, Sai Surya Vamsi Krishna </t>
+  </si>
+  <si>
+    <t>S, Sethurajesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhiram, Jayanthi Abhiram </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benny Roshini, Chelashia Mickle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kandepu, Kandepu Venkata Dinesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nayak, Chandini Mayee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pothamsetty, Adithya Vardhan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aravapalli, Sai Venkata Naga Prasannakumar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buddhana, Nitin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mangavalli, pavan kumar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakhineti, Mounisha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chavali, sridhar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katikala, Sudheer Kumar </t>
+  </si>
+  <si>
+    <t>Matlapudi, Pavaneswar Satya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samanthakurthi, Nitish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanuboddi, Yashwanth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chunchu, Rakesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kakumanu, Lakshmi Pranav </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khanduri, Shubham </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohammad, Khaja Moinuddin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philip, Ajeesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravi, Srihitha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">singh, Kaushlendra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thondepu, Venkata Lakshmi Neeraja </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +829,41 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -529,7 +880,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -552,11 +903,265 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,6 +1177,104 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,20 +1555,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80268717-6C28-4DD7-8817-C5C41B472DC1}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.71875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>145</v>
       </c>
@@ -879,7 +1584,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -892,14 +1597,65 @@
       <c r="D2" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <f>D2/5</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>151</v>
       </c>
       <c r="D3" s="6">
         <f>SUM(D2:D2)</f>
         <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="1">
+        <v>125</v>
+      </c>
+      <c r="E7" s="1">
+        <f>D7/5</f>
+        <v>25</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44648</v>
+      </c>
+      <c r="G7" s="7">
+        <v>44687</v>
       </c>
     </row>
   </sheetData>
@@ -911,17 +1667,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.32421875" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>143</v>
       </c>
@@ -929,941 +1685,941 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B51" s="3"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B52" s="3"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B86" s="3"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B92" s="3"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B95" s="3"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B103" s="3"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B115" s="3"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B129" s="3"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B141" s="3"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="3"/>
       <c r="B143" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="3"/>
       <c r="B144" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B150" s="3"/>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B155" s="3"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="3"/>
       <c r="B156" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="3"/>
       <c r="B157" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="3"/>
       <c r="B158" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="3"/>
       <c r="B159" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="3"/>
       <c r="B160" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="3"/>
       <c r="B161" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="3"/>
       <c r="B162" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="3"/>
       <c r="B163" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="3"/>
       <c r="B164" s="3" t="s">
         <v>142</v>
@@ -1873,4 +2629,1803 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6FDBA4-15D2-464A-AB13-F453285B6638}">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="7">
+        <v>44648</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="7">
+        <v>44649</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="7">
+        <v>44650</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="7">
+        <v>44651</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="7">
+        <v>44652</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="9">
+        <v>44653</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="9">
+        <v>44654</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="7">
+        <v>44655</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="7">
+        <v>44656</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="7">
+        <v>44657</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44658</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" s="9">
+        <v>44659</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="9">
+        <v>44660</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="9">
+        <v>44661</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="9">
+        <v>44662</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" s="7">
+        <v>44663</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="7">
+        <v>44664</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="9">
+        <v>44665</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="9">
+        <v>44666</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="9">
+        <v>44667</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="9">
+        <v>44668</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" s="7">
+        <v>44669</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="7">
+        <v>44670</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="7">
+        <v>44671</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="7">
+        <v>44672</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E27" s="7">
+        <v>44673</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="E28" s="9">
+        <v>44674</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="9">
+        <v>44675</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="7">
+        <v>44676</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E31" s="7">
+        <v>44677</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" s="7">
+        <v>44678</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="7">
+        <v>44679</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H33" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="7">
+        <v>44680</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" s="9">
+        <v>44681</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="9">
+        <v>44682</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="7">
+        <v>44683</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H37" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E38" s="9">
+        <v>44684</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="7">
+        <v>44685</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="11">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E40" s="7">
+        <v>44686</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H40" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="11">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="7">
+        <v>44687</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D28:D29"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8C0980-CA55-4170-A070-C42E91BC641F}">
+  <dimension ref="A1:T29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="41"/>
+    </row>
+    <row r="2" spans="1:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="36"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="32"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="18"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="18"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="18"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="18"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="18"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="18"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="18"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="18"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>10</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="18"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="18"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="18"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>13</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="18"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="18"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>15</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="18"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>16</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="18"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>17</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="18"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>18</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="18"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>19</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="18"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>20</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="18"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>21</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="18"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>22</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="18"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>23</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="18"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>24</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="18"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>25</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="18"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>26</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="18"/>
+    </row>
+    <row r="29" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="23">
+        <v>27</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>